<commit_message>
<build>: add download function of clim_extract.
</commit_message>
<xml_diff>
--- a/tests/testthat/datatest.xlsx
+++ b/tests/testthat/datatest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czhxu\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\climplot\climplot\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01ACAB00-BCA2-46B6-936A-9DC71B78DC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB3542C-D9F8-4A98-B51A-CCB238C3F8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01181A9A-6335-46EA-A76E-000E0A881763}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,10 +53,6 @@
   </si>
   <si>
     <t>altitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -429,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5616DC0F-A6E8-43E0-8164-4F905A4406EE}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -462,13 +458,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>113.56</v>
+        <v>112.15</v>
       </c>
       <c r="D2">
-        <v>23.12</v>
+        <v>22</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -479,30 +475,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>112.15</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>22</v>
+        <v>-30</v>
       </c>
       <c r="E3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>116</v>
-      </c>
-      <c r="D4">
-        <v>40</v>
-      </c>
-      <c r="E4">
-        <v>1000</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>